<commit_message>
modified:   accuracy.ipynb modified:   cumulative_accuracy.ipynb modified:   future.xlsx
</commit_message>
<xml_diff>
--- a/future.xlsx
+++ b/future.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkdb\OneDrive\Desktop\ballgorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41663CE-D3D6-4A63-B97A-83981C6D9CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D03D277-2AB9-4418-8231-12337C1480E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2453" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2468" uniqueCount="138">
   <si>
     <t>Date</t>
   </si>
@@ -613,11 +613,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4069,7 +4069,7 @@
   <dimension ref="A1:N274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="D210" sqref="D210"/>
+      <selection activeCell="H202" sqref="H202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11484,7 +11484,7 @@
         <v>98</v>
       </c>
       <c r="M161" s="7">
-        <f t="shared" ref="M161:M206" si="5">ABS(D161-F161)</f>
+        <f t="shared" ref="M161:M209" si="5">ABS(D161-F161)</f>
         <v>3</v>
       </c>
       <c r="N161" t="b">
@@ -11718,7 +11718,7 @@
         <v>6</v>
       </c>
       <c r="N166" t="b">
-        <f t="shared" ref="N166:N206" si="6">K166=I166</f>
+        <f t="shared" ref="N166:N209" si="6">K166=I166</f>
         <v>1</v>
       </c>
     </row>
@@ -13572,11 +13572,40 @@
       <c r="C207" t="s">
         <v>41</v>
       </c>
+      <c r="D207" s="7">
+        <v>110</v>
+      </c>
       <c r="E207" t="s">
         <v>51</v>
       </c>
+      <c r="F207" s="7">
+        <v>113</v>
+      </c>
+      <c r="G207" t="s">
+        <v>15</v>
+      </c>
       <c r="H207" t="s">
         <v>86</v>
+      </c>
+      <c r="I207" t="s">
+        <v>51</v>
+      </c>
+      <c r="J207" t="s">
+        <v>41</v>
+      </c>
+      <c r="K207" t="s">
+        <v>41</v>
+      </c>
+      <c r="L207" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="M207" s="7">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N207" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:14" x14ac:dyDescent="0.45">
@@ -13589,14 +13618,43 @@
       <c r="C208" t="s">
         <v>82</v>
       </c>
+      <c r="D208" s="7">
+        <v>140</v>
+      </c>
       <c r="E208" t="s">
         <v>54</v>
       </c>
+      <c r="F208" s="7">
+        <v>137</v>
+      </c>
+      <c r="G208" t="s">
+        <v>15</v>
+      </c>
       <c r="H208" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I208" t="s">
+        <v>82</v>
+      </c>
+      <c r="J208" t="s">
+        <v>54</v>
+      </c>
+      <c r="K208" t="s">
+        <v>54</v>
+      </c>
+      <c r="L208" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="M208" s="7">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="N208" t="b">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A209" s="3" t="s">
         <v>119</v>
       </c>
@@ -13606,14 +13664,43 @@
       <c r="C209" t="s">
         <v>58</v>
       </c>
+      <c r="D209" s="7">
+        <v>128</v>
+      </c>
       <c r="E209" t="s">
         <v>33</v>
       </c>
+      <c r="F209" s="7">
+        <v>91</v>
+      </c>
+      <c r="G209" t="s">
+        <v>15</v>
+      </c>
       <c r="H209" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I209" t="s">
+        <v>58</v>
+      </c>
+      <c r="J209" t="s">
+        <v>33</v>
+      </c>
+      <c r="K209" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="L209" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="M209" s="7">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="N209" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A210" s="3" t="s">
         <v>120</v>
       </c>
@@ -13630,7 +13717,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A211" s="3" t="s">
         <v>120</v>
       </c>
@@ -13647,7 +13734,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="212" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A212" s="3" t="s">
         <v>120</v>
       </c>
@@ -13664,7 +13751,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A213" s="3" t="s">
         <v>120</v>
       </c>
@@ -13681,7 +13768,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A214" s="3" t="s">
         <v>120</v>
       </c>
@@ -13698,7 +13785,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A215" s="3" t="s">
         <v>120</v>
       </c>
@@ -13715,7 +13802,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="216" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A216" s="3" t="s">
         <v>120</v>
       </c>
@@ -13732,7 +13819,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="217" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A217" s="3" t="s">
         <v>120</v>
       </c>
@@ -13749,7 +13836,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="218" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A218" s="3" t="s">
         <v>120</v>
       </c>
@@ -13766,7 +13853,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="219" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A219" s="3" t="s">
         <v>120</v>
       </c>
@@ -13783,7 +13870,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="220" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A220" s="3" t="s">
         <v>120</v>
       </c>
@@ -13800,7 +13887,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="221" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A221" s="3" t="s">
         <v>120</v>
       </c>
@@ -13817,7 +13904,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="222" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A222" s="3" t="s">
         <v>121</v>
       </c>
@@ -13834,7 +13921,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="223" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A223" s="3" t="s">
         <v>121</v>
       </c>
@@ -13851,7 +13938,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="224" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A224" s="3" t="s">
         <v>121</v>
       </c>
@@ -15558,27 +15645,27 @@
       </c>
       <c r="B29" s="9">
         <f>COUNTIFS(Sheet1!$L:$L,Sheet2!$B$1,Sheet1!$A:$A,Sheet2!$A29)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" s="9">
         <f>COUNTIFS(Sheet1!$L:$L,Sheet2!$C$1,Sheet1!$A:$A,Sheet2!$A29)</f>
-        <v>0</v>
-      </c>
-      <c r="D29" s="10" t="str">
+        <v>2</v>
+      </c>
+      <c r="D29" s="10">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="E29" s="14" t="str">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E29" s="14">
         <f>IFERROR(AVERAGEIFS(Sheet1!$M$2:$M$500, Sheet1!$A$2:$A$500, A29, Sheet1!$L$2:$L$500, "Yes"),"")</f>
-        <v/>
-      </c>
-      <c r="F29" s="14" t="str">
+        <v>37</v>
+      </c>
+      <c r="F29" s="14">
         <f>IFERROR(AVERAGEIFS(Sheet1!$M$2:$M$500, Sheet1!$A$2:$A$500, A29, Sheet1!$L$2:$L$500, "No"),"")</f>
-        <v/>
+        <v>3</v>
       </c>
       <c r="G29" s="16" cm="1">
         <f t="array" ref="G29">SUM(($B$2:B29)/SUM($B$2:C29))</f>
-        <v>0.48292682926829283</v>
+        <v>0.48076923076923084</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.45">
@@ -15607,7 +15694,7 @@
       </c>
       <c r="G30" s="16" cm="1">
         <f t="array" ref="G30">SUM(($B$2:B30)/SUM($B$2:C30))</f>
-        <v>0.48292682926829283</v>
+        <v>0.48076923076923084</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.45">
@@ -15636,7 +15723,7 @@
       </c>
       <c r="G31" s="16" cm="1">
         <f t="array" ref="G31">SUM(($B$2:B31)/SUM($B$2:C31))</f>
-        <v>0.48292682926829283</v>
+        <v>0.48076923076923084</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.45">
@@ -15665,7 +15752,7 @@
       </c>
       <c r="G32" s="16" cm="1">
         <f t="array" ref="G32">SUM(($B$2:B32)/SUM($B$2:C32))</f>
-        <v>0.48292682926829283</v>
+        <v>0.48076923076923084</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.45">
@@ -15694,7 +15781,7 @@
       </c>
       <c r="G33" s="16" cm="1">
         <f t="array" ref="G33">SUM(($B$2:B33)/SUM($B$2:C33))</f>
-        <v>0.48292682926829283</v>
+        <v>0.48076923076923084</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.45">
@@ -15723,7 +15810,7 @@
       </c>
       <c r="G34" s="16" cm="1">
         <f t="array" ref="G34">SUM(($B$2:B34)/SUM($B$2:C34))</f>
-        <v>0.48292682926829283</v>
+        <v>0.48076923076923084</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.45">
@@ -15752,7 +15839,7 @@
       </c>
       <c r="G35" s="16" cm="1">
         <f t="array" ref="G35">SUM(($B$2:B35)/SUM($B$2:C35))</f>
-        <v>0.48292682926829283</v>
+        <v>0.48076923076923084</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.45">
@@ -15781,7 +15868,7 @@
       </c>
       <c r="G36" s="16" cm="1">
         <f t="array" ref="G36">SUM(($B$2:B36)/SUM($B$2:C36))</f>
-        <v>0.48292682926829283</v>
+        <v>0.48076923076923084</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.45">
@@ -15810,7 +15897,7 @@
       </c>
       <c r="G37" s="16" cm="1">
         <f t="array" ref="G37">SUM(($B$2:B37)/SUM($B$2:C37))</f>
-        <v>0.48292682926829283</v>
+        <v>0.48076923076923084</v>
       </c>
     </row>
   </sheetData>
@@ -15869,19 +15956,19 @@
       <c r="A1" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="18"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="19">
         <v>0.37815126050420172</v>
       </c>
     </row>
@@ -15889,10 +15976,10 @@
       <c r="A3" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>0.58695652173913038</v>
       </c>
     </row>

</xml_diff>